<commit_message>
Custom waste spreading by category and activity (part 2)
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/nace_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/nace_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24400" yWindow="4180" windowWidth="25260" windowHeight="13700" tabRatio="500"/>
+    <workbookView xWindow="2500" yWindow="1600" windowWidth="32780" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,13 +195,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,18 +491,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="128" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="112.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Added an excel file for the treatement full names
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/nace_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/nace_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1600" windowWidth="32780" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="1220" windowWidth="32780" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="128" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Rexport XLS to CSV
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/nace_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/nace_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1220" windowWidth="32780" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="2920" yWindow="2140" windowWidth="20040" windowHeight="13120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="128" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>